<commit_message>
시연 동영상 테스트 용 (노드 : 40, lower : 23,0.01, upper : 36,360, draft : 15, population : 200, max_evalu : 10000)
</commit_message>
<xml_diff>
--- a/Dataset/testxl.xlsx
+++ b/Dataset/testxl.xlsx
@@ -39,15 +39,15 @@
     <t>WaveDirection</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>Draught</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Speed2</t>
+    <t>time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Draught</t>
+    <t>Speed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -397,18 +397,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -429,7 +429,7 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">

</xml_diff>